<commit_message>
modified:   data/data.xlsx 	modified:   modules/__pycache__/create_source.cpython-310.pyc 	modified:   modules/__pycache__/proxy.cpython-310.pyc 	modified:   modules/__pycache__/scraper.cpython-310.pyc 	modified:   test.py
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,37 +476,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Xiaomi Mi Band 7</t>
+          <t>Onvo OV50F900 Frameless 4K Ultra HD 50" 127 Ekran Uydu Alıcılı Android Smart LED TV</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Trendyol </t>
+          <t xml:space="preserve">Trendyol/Beyaz Live </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>698,99 TL</t>
+          <t>5.649,00 TL</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pttavm/Koycebine </t>
+          <t xml:space="preserve">Trendyol/Kargomarket </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>779,00 TL</t>
+          <t>5.689,00 TL</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10.40</t>
+          <t>0.70</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.akakce.com/akilli-bileklik/en-ucuz-xiaomi-mi-band-7-fiyati,1708200663.html</t>
+          <t>https://www.akakce.com/televizyon/en-ucuz-onvo-onvo-ov50f900-127-cm-frameless-4k-uhd-lisansli-android-smart-bluetooth-dahili-uydu-alicili-1000-hz-fiyati,1623302352.html</t>
         </is>
       </c>
     </row>
@@ -516,37 +516,237 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LG 50QNED7S6QA 4K Ultra HD 50" 127 Ekran Uydu Alıcılı Smart QNED TV</t>
+          <t>Huawei MateBook D16 i5-12450H 8 GB 512 GB SSD UHD Graphics 16" Notebook</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Trendyol/doludepo </t>
+          <t xml:space="preserve">Trendyol/HIZLIALTEKNOLOJI </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13.799,00 TL</t>
+          <t>15.599,00 TL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teknosa.com/doludepo </t>
+          <t xml:space="preserve">Trendyol/Central Teknoloji </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>13.869,00 TL</t>
+          <t>15.629,00 TL</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.50</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.akakce.com/televizyon/en-ucuz-lg-50qned7s6-50-127-ekran-uydu-alicili-4k-ultra-hd-webos-smart-qned-tv-fiyati,84783208.html</t>
+          <t>https://www.akakce.com/laptop-notebook/en-ucuz-huawei-matebook-d16-i5-12450h-8-gb-512-gb-ssd-uhd-graphics-16-notebook-fiyati,1954151588.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sapphire NITRO+ AMD RX 6700 XT 11306-01-20G 192 Bit GDDR6 12 GB Ekran Kartı</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sinerji Bilgisayar </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8.899,17 TL</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trendyol/Dali Teknoloji </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10.499,00 TL</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>15.24</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://www.akakce.com/ekran-karti/en-ucuz-sapphire-nitro-amd-rx-6700-xt-11306-01-20g-192-bit-gddr6-12-gb-fiyati,1100803768.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lenovo Ideapad 3 82H802RKTX i3-1115G4 8 GB 256 GB SSD UHD Graphıcs 15.6" Full HD Notebook</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trendyol/Teknosa </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>7.995,00 TL</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trendyol/VATAN BİLGİSAYAR </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>7.999,00 TL</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://www.akakce.com/laptop-notebook/en-ucuz-lenovo-ideapad-3-82h802rktx-i3-1115g4-8-gb-256-gb-ssd-uhd-graphics-15-6-full-hd-notebook-fiyati,2110900082.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LG 55QNED7S6QA 4K Ultra HD 55" 140 Ekran Uydu Alıcılı Smart QNED TV</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pttavm/KIRMIZI ELMA </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>16.619,00 TL</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trendyol/Teknomix </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>16.865,00 TL</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.46</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://www.akakce.com/televizyon/en-ucuz-lg-55qned7s6-55inc-139-cm-4k-uhd-webos-smart-tv-uydu-alicili-fiyati,85415069.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Daikin MC70L Hava Temizleme Cihazı</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">N11/basaranstore </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3.707,95 TL</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Veyisoglugrup.com 9,9 490 Yorum</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3.749,00 TL</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://www.akakce.com/hava-temizleme-cihazi/en-ucuz-daikin-mc70l-fiyati,833500.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sony A7 III Body Aynasız Fotoğraf Makinesi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hepsiburada/FOTO ÇARŞI </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>32.148,00 TL</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Klas Foto 8,7 26 Yorum</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>32.499,00 TL</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://www.akakce.com/fotograf-makinesi/en-ucuz-sony-a7-iii-body-fiyati,209457498.html</t>
         </is>
       </c>
     </row>

</xml_diff>